<commit_message>
Ahi ta corregido lo de la base
</commit_message>
<xml_diff>
--- a/Documentacion/Base de datos/Relacional Base de datos.xlsx
+++ b/Documentacion/Base de datos/Relacional Base de datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\EstacionamientosVIP\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Parkplatz\Documentacion\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -425,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D22:D26" totalsRowShown="0">
-  <autoFilter ref="D22:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D23:D27" totalsRowShown="0">
+  <autoFilter ref="D23:D27"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Cordenadas"/>
   </tableColumns>
@@ -495,8 +495,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="D2:D8" totalsRowShown="0">
-  <autoFilter ref="D2:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="D2:D7" totalsRowShown="0">
+  <autoFilter ref="D2:D7"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Datos"/>
   </tableColumns>
@@ -505,8 +505,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="F2:F10" totalsRowShown="0">
-  <autoFilter ref="F2:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="H11:H19" totalsRowShown="0">
+  <autoFilter ref="H11:H19"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Datos Estacionamiento"/>
   </tableColumns>
@@ -535,8 +535,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="D11:D15" totalsRowShown="0">
-  <autoFilter ref="D11:D15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="D10:D14" totalsRowShown="0">
+  <autoFilter ref="D10:D14"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Servicios"/>
   </tableColumns>
@@ -565,8 +565,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D17:D20" totalsRowShown="0">
-  <autoFilter ref="D17:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D16:D20" totalsRowShown="0">
+  <autoFilter ref="D16:D20"/>
   <tableColumns count="1">
     <tableColumn id="1" name="estacionamiento"/>
   </tableColumns>
@@ -840,7 +840,7 @@
   <dimension ref="B2:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.85546875" customWidth="1"/>
   </cols>
@@ -860,9 +860,6 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
         <v>48</v>
       </c>
@@ -874,9 +871,6 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
       <c r="H3" t="s">
         <v>49</v>
       </c>
@@ -888,9 +882,6 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
         <v>50</v>
       </c>
@@ -902,9 +893,6 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
       <c r="H5" t="s">
         <v>51</v>
       </c>
@@ -916,9 +904,6 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
       <c r="H6" t="s">
         <v>52</v>
       </c>
@@ -928,22 +913,13 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
       <c r="H8" t="s">
         <v>53</v>
       </c>
@@ -952,16 +928,13 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>40</v>
+      <c r="D10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -969,15 +942,21 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -985,10 +964,13 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -996,56 +978,74 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
       <c r="F15" t="s">
         <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>26</v>
       </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
       <c r="F16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -1064,55 +1064,55 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>29</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -1183,8 +1183,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="17">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1201,6 +1201,7 @@
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Subo la base corregida en excel
</commit_message>
<xml_diff>
--- a/Documentacion/Base de datos/Relacional Base de datos.xlsx
+++ b/Documentacion/Base de datos/Relacional Base de datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Parkplatz\Documentacion\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Documents\GitHub\Parkplatz\Documentacion\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos1" hidden="1">zigma.articulos</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos" hidden="1">zigma.articulos</definedName>
     <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos11" hidden="1">zigma.articulos</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1" hidden="1">zigma.tipocontenido</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios1" hidden="1">zigma.usuarios</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido" hidden="1">zigma.tipocontenido</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios" hidden="1">zigma.usuarios</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -46,7 +46,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma articulos-c8b0c243-cbd7-4c96-8940-03d9780a04ae">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -64,7 +64,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma tipocontenido-deb04f1f-f5a3-4d99-abc3-4dd1f12dd360">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -73,7 +73,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma usuarios-a4f0877f-852b-46cb-b346-8dc8bdac1ada">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>nombre</t>
   </si>
@@ -425,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D23:D27" totalsRowShown="0">
-  <autoFilter ref="D23:D27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D22:D26" totalsRowShown="0">
+  <autoFilter ref="D22:D26"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Cordenadas"/>
   </tableColumns>
@@ -495,8 +495,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="D2:D7" totalsRowShown="0">
-  <autoFilter ref="D2:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="D2:D6" totalsRowShown="0">
+  <autoFilter ref="D2:D6"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Datos"/>
   </tableColumns>
@@ -535,8 +535,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="D10:D14" totalsRowShown="0">
-  <autoFilter ref="D10:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="D9:D13" totalsRowShown="0">
+  <autoFilter ref="D9:D13"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Servicios"/>
   </tableColumns>
@@ -565,8 +565,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D16:D20" totalsRowShown="0">
-  <autoFilter ref="D16:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D15:D19" totalsRowShown="0">
+  <autoFilter ref="D15:D19"/>
   <tableColumns count="1">
     <tableColumn id="1" name="estacionamiento"/>
   </tableColumns>
@@ -840,7 +840,7 @@
   <dimension ref="B2:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,9 +912,6 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
       <c r="H7" t="s">
         <v>54</v>
       </c>
@@ -928,13 +925,16 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
@@ -964,7 +964,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
@@ -977,9 +977,6 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
@@ -991,6 +988,9 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
       <c r="F15" t="s">
         <v>2</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
         <v>43</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
         <v>44</v>
@@ -1028,7 +1028,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
@@ -1039,7 +1039,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H19" t="s">
         <v>40</v>
@@ -1049,9 +1049,6 @@
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
       <c r="F20" t="s">
         <v>46</v>
       </c>
@@ -1065,6 +1062,9 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
       <c r="F22" t="s">
         <v>47</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1098,16 +1098,13 @@
         <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
       <c r="G27" s="2" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Subo la base actualizada y los pocos diccionarios de datos
</commit_message>
<xml_diff>
--- a/Documentacion/Base de datos/Relacional Base de datos.xlsx
+++ b/Documentacion/Base de datos/Relacional Base de datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Documents\GitHub\Parkplatz\Documentacion\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Parkplatz\Documentacion\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos" hidden="1">zigma.articulos</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos1" hidden="1">zigma.articulos</definedName>
     <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos11" hidden="1">zigma.articulos</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido" hidden="1">zigma.tipocontenido</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios" hidden="1">zigma.usuarios</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1" hidden="1">zigma.tipocontenido</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios1" hidden="1">zigma.usuarios</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -46,7 +46,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma articulos-c8b0c243-cbd7-4c96-8940-03d9780a04ae">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -64,7 +64,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma tipocontenido-deb04f1f-f5a3-4d99-abc3-4dd1f12dd360">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -73,7 +73,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma usuarios-a4f0877f-852b-46cb-b346-8dc8bdac1ada">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>nombre</t>
   </si>
@@ -425,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D22:D26" totalsRowShown="0">
-  <autoFilter ref="D22:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="D21:D25" totalsRowShown="0">
+  <autoFilter ref="D21:D25"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Cordenadas"/>
   </tableColumns>
@@ -565,8 +565,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D15:D19" totalsRowShown="0">
-  <autoFilter ref="D15:D19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="D15:D18" totalsRowShown="0">
+  <autoFilter ref="D15:D18"/>
   <tableColumns count="1">
     <tableColumn id="1" name="estacionamiento"/>
   </tableColumns>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,9 +1038,6 @@
       <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
       <c r="H19" t="s">
         <v>40</v>
       </c>
@@ -1057,13 +1054,16 @@
       <c r="B21" t="s">
         <v>31</v>
       </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
         <v>47</v>
@@ -1074,7 +1074,7 @@
         <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1090,15 +1090,12 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Unas pequeñas modificaciones a la base
</commit_message>
<xml_diff>
--- a/Documentacion/Base de datos/Relacional Base de datos.xlsx
+++ b/Documentacion/Base de datos/Relacional Base de datos.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos1" hidden="1">zigma.articulos</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos" hidden="1">zigma.articulos</definedName>
     <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos11" hidden="1">zigma.articulos</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1" hidden="1">zigma.tipocontenido</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios1" hidden="1">zigma.usuarios</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido" hidden="1">zigma.tipocontenido</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios" hidden="1">zigma.usuarios</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -46,7 +46,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma articulos-c8b0c243-cbd7-4c96-8940-03d9780a04ae">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -64,7 +64,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma tipocontenido-deb04f1f-f5a3-4d99-abc3-4dd1f12dd360">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -73,7 +73,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma usuarios-a4f0877f-852b-46cb-b346-8dc8bdac1ada">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios1"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>nombre</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Cordenadas</t>
+  </si>
+  <si>
+    <t>Piso</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla17" displayName="Tabla17" ref="B18:B21" totalsRowShown="0">
-  <autoFilter ref="B18:B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla17" displayName="Tabla17" ref="B18:B22" totalsRowShown="0">
+  <autoFilter ref="B18:B22"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Lugares"/>
   </tableColumns>
@@ -465,8 +468,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabla22" displayName="Tabla22" ref="B23:B26" totalsRowShown="0">
-  <autoFilter ref="B23:B26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabla22" displayName="Tabla22" ref="B24:B27" totalsRowShown="0">
+  <autoFilter ref="B24:B27"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Favoritos"/>
   </tableColumns>
@@ -475,8 +478,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabla23" displayName="Tabla23" ref="B28:B31" totalsRowShown="0">
-  <autoFilter ref="B28:B31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabla23" displayName="Tabla23" ref="B29:B32" totalsRowShown="0">
+  <autoFilter ref="B29:B32"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Catalogo modo lugares"/>
   </tableColumns>
@@ -485,8 +488,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabla24" displayName="Tabla24" ref="B33:B37" totalsRowShown="0">
-  <autoFilter ref="B33:B37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabla24" displayName="Tabla24" ref="B34:B38" totalsRowShown="0">
+  <autoFilter ref="B34:B38"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Recientes"/>
   </tableColumns>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H37"/>
+  <dimension ref="B2:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,6 +1065,9 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
@@ -1070,16 +1076,13 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
       <c r="D23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -1087,7 +1090,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
@@ -1095,21 +1098,21 @@
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
       <c r="E28" t="s">
         <v>38</v>
       </c>
@@ -1119,7 +1122,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
         <v>36</v>
@@ -1127,7 +1130,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
@@ -1135,20 +1138,22 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
       <c r="E33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
         <v>35</v>
@@ -1156,7 +1161,7 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
@@ -1164,7 +1169,7 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
@@ -1172,6 +1177,11 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subo proyecto web y actualizo db y documentacion
</commit_message>
<xml_diff>
--- a/Documentacion/Base de datos/Relacional Base de datos.xlsx
+++ b/Documentacion/Base de datos/Relacional Base de datos.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos" hidden="1">zigma.articulos</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos1" hidden="1">zigma.articulos</definedName>
     <definedName name="_xlcn.ModelConnection_For_Libro1zigma.articulos11" hidden="1">zigma.articulos</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido" hidden="1">zigma.tipocontenido</definedName>
-    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios" hidden="1">zigma.usuarios</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1" hidden="1">zigma.tipocontenido</definedName>
+    <definedName name="_xlcn.ModelConnection_For_Libro1zigma.usuarios1" hidden="1">zigma.usuarios</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -46,7 +46,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma articulos-c8b0c243-cbd7-4c96-8940-03d9780a04ae">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.articulos1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -64,7 +64,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma tipocontenido-deb04f1f-f5a3-4d99-abc3-4dd1f12dd360">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.tipocontenido1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -73,7 +73,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="zigma usuarios-a4f0877f-852b-46cb-b346-8dc8bdac1ada">
-          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios"/>
+          <x15:rangePr sourceName="_xlcn.ModelConnection_For_Libro1zigma.usuarios1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>nombre</t>
   </si>
@@ -280,6 +280,27 @@
   </si>
   <si>
     <t>Piso</t>
+  </si>
+  <si>
+    <t>rel_tipousuario_menu</t>
+  </si>
+  <si>
+    <t>idTipoUsuario</t>
+  </si>
+  <si>
+    <t>idMenu</t>
+  </si>
+  <si>
+    <t>catMenu</t>
+  </si>
+  <si>
+    <t>nombreCampo</t>
+  </si>
+  <si>
+    <t>tipoCampo</t>
+  </si>
+  <si>
+    <t>nombreAMostrar</t>
   </si>
 </sst>
 </file>
@@ -492,6 +513,26 @@
   <autoFilter ref="B34:B38"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Recientes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="G30:G32" totalsRowShown="0">
+  <autoFilter ref="G30:G32"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="rel_tipousuario_menu"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G34:G38" totalsRowShown="0">
+  <autoFilter ref="G34:G38"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="catMenu"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +893,7 @@
     <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
     <col min="8" max="8" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1135,60 +1176,84 @@
       <c r="E30" t="s">
         <v>30</v>
       </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>57</v>
       </c>
       <c r="E34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>59</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>24</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="17">
+  <tableParts count="19">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1206,6 +1271,8 @@
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
     <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>